<commit_message>
modified 68 bus system
</commit_message>
<xml_diff>
--- a/system_cases/NETSNYPS68bus/NETS_NYPS_68_modified2.xlsx
+++ b/system_cases/NETSNYPS68bus/NETS_NYPS_68_modified2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Simplus-Grid-Tool\system_cases\NETSNYPS68bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F76D9F-8453-4DAF-A058-E1B6841235CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D6BE5B-FD20-47FA-9AFE-F1DD8590D72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="3180" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -585,6 +585,27 @@
   </si>
   <si>
     <t>GFM</t>
+  </si>
+  <si>
+    <t>Sbase</t>
+  </si>
+  <si>
+    <t>GFL</t>
+  </si>
+  <si>
+    <t>V_dc</t>
+  </si>
+  <si>
+    <t>C_dc</t>
+  </si>
+  <si>
+    <t>f_v_dc</t>
+  </si>
+  <si>
+    <t>f_pll</t>
+  </si>
+  <si>
+    <t>f_i_dq</t>
   </si>
 </sst>
 </file>
@@ -595,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +768,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -763,19 +789,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,6 +802,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -814,22 +840,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -839,48 +857,72 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -1218,10 +1260,10 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="6">
@@ -1233,7 +1275,7 @@
       <c r="E3" s="6">
         <v>40</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <v>0</v>
       </c>
       <c r="G3" s="6">
@@ -1256,22 +1298,22 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="18">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="14">
         <v>0.98</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="15">
         <v>3.45</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="14">
         <v>0</v>
       </c>
       <c r="G4" s="7">
@@ -1294,13 +1336,13 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="18">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>0.98299999999999998</v>
       </c>
       <c r="D5" s="7">
@@ -1309,7 +1351,7 @@
       <c r="E5" s="7">
         <v>6.5</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="14">
         <v>0</v>
       </c>
       <c r="G5" s="7">
@@ -1332,13 +1374,13 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="18">
+      <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>0.997</v>
       </c>
       <c r="D6" s="7">
@@ -1347,7 +1389,7 @@
       <c r="E6" s="7">
         <v>6.32</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="14">
         <v>0</v>
       </c>
       <c r="G6" s="7">
@@ -1370,13 +1412,13 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="14">
         <v>2</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <v>1.0109999999999999</v>
       </c>
       <c r="D7" s="7">
@@ -1385,7 +1427,7 @@
       <c r="E7" s="7">
         <v>5.05</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="14">
         <v>0</v>
       </c>
       <c r="G7" s="7">
@@ -1408,13 +1450,13 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="18">
+      <c r="A8" s="14">
         <v>6</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>1.05</v>
       </c>
       <c r="D8" s="7">
@@ -1423,7 +1465,7 @@
       <c r="E8" s="7">
         <v>7</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="14">
         <v>0</v>
       </c>
       <c r="G8" s="7">
@@ -1446,13 +1488,13 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>7</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="14">
         <v>2</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>1.0629999999999999</v>
       </c>
       <c r="D9" s="7">
@@ -1461,7 +1503,7 @@
       <c r="E9" s="7">
         <v>5.6</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="14">
         <v>0</v>
       </c>
       <c r="G9" s="7">
@@ -1484,13 +1526,13 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="18">
+      <c r="A10" s="14">
         <v>8</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <v>2</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <v>1.03</v>
       </c>
       <c r="D10" s="7">
@@ -1499,7 +1541,7 @@
       <c r="E10" s="7">
         <v>5.4</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="14">
         <v>0</v>
       </c>
       <c r="G10" s="7">
@@ -1522,22 +1564,22 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="18">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="14">
         <v>2</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <v>1.0249999999999999</v>
       </c>
       <c r="D11" s="7">
         <v>0</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="15">
         <v>2</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="14">
         <v>0</v>
       </c>
       <c r="G11" s="7">
@@ -1560,13 +1602,13 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="18">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="14">
         <v>2</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
         <v>1.01</v>
       </c>
       <c r="D12" s="7">
@@ -1575,7 +1617,7 @@
       <c r="E12" s="7">
         <v>5</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="14">
         <v>0</v>
       </c>
       <c r="G12" s="7">
@@ -1598,13 +1640,13 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="18">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="14">
         <v>2</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="7">
@@ -1613,7 +1655,7 @@
       <c r="E13" s="7">
         <v>10</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="14">
         <v>0</v>
       </c>
       <c r="G13" s="7">
@@ -1636,22 +1678,22 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="18">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="24">
         <v>3</v>
       </c>
-      <c r="C14" s="39">
-        <v>1</v>
-      </c>
-      <c r="D14" s="40">
-        <v>0</v>
-      </c>
-      <c r="E14" s="41">
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
         <v>2</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="24">
         <v>0</v>
       </c>
       <c r="G14" s="7">
@@ -1674,22 +1716,22 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="18">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="14">
         <v>2</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="14">
         <v>1.0109999999999999</v>
       </c>
       <c r="D15" s="7">
         <v>0</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="29">
         <v>27.91</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="14">
         <v>0</v>
       </c>
       <c r="G15" s="7">
@@ -1712,10 +1754,10 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="18">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="14">
         <v>2</v>
       </c>
       <c r="C16" s="7">
@@ -1727,7 +1769,7 @@
       <c r="E16" s="7">
         <v>17.850000000000001</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="14">
         <v>0</v>
       </c>
       <c r="G16" s="7">
@@ -1750,13 +1792,13 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="18">
+      <c r="A17" s="14">
         <v>15</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="14">
         <v>2</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <v>1</v>
       </c>
       <c r="D17" s="7">
@@ -1765,7 +1807,7 @@
       <c r="E17" s="7">
         <v>10</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="14">
         <v>0</v>
       </c>
       <c r="G17" s="7">
@@ -1788,13 +1830,13 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="17">
+      <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="13">
         <v>2</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="13">
         <v>1.0449999999999999</v>
       </c>
       <c r="D18" s="6">
@@ -1803,7 +1845,7 @@
       <c r="E18" s="6">
         <v>2.5</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="13">
         <v>0</v>
       </c>
       <c r="G18" s="6">
@@ -1826,22 +1868,22 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="18">
+      <c r="A19" s="14">
         <v>17</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="14">
         <v>3</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="14">
         <v>1</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="15">
         <v>4</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="14">
         <v>0</v>
       </c>
       <c r="G19" s="7">
@@ -1864,10 +1906,10 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="18">
+      <c r="A20" s="14">
         <v>18</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="14">
         <v>3</v>
       </c>
       <c r="C20" s="7">
@@ -1879,7 +1921,7 @@
       <c r="E20" s="7">
         <v>0</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="14">
         <v>0</v>
       </c>
       <c r="G20" s="7">
@@ -1902,13 +1944,13 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="18">
+      <c r="A21" s="14">
         <v>19</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="14">
         <v>3</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="14">
         <v>1</v>
       </c>
       <c r="D21" s="7">
@@ -1917,7 +1959,7 @@
       <c r="E21" s="7">
         <v>0</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="14">
         <v>0</v>
       </c>
       <c r="G21" s="7">
@@ -1940,10 +1982,10 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="18">
+      <c r="A22" s="14">
         <v>20</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="14">
         <v>3</v>
       </c>
       <c r="C22" s="7">
@@ -1955,7 +1997,7 @@
       <c r="E22" s="7">
         <v>0</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="14">
         <v>0</v>
       </c>
       <c r="G22" s="7">
@@ -1978,13 +2020,13 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="18">
+      <c r="A23" s="14">
         <v>21</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="14">
         <v>3</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="14">
         <v>1</v>
       </c>
       <c r="D23" s="7">
@@ -1993,7 +2035,7 @@
       <c r="E23" s="7">
         <v>0</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="14">
         <v>0</v>
       </c>
       <c r="G23" s="7">
@@ -2016,10 +2058,10 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="18">
+      <c r="A24" s="14">
         <v>22</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="14">
         <v>3</v>
       </c>
       <c r="C24" s="7">
@@ -2031,7 +2073,7 @@
       <c r="E24" s="7">
         <v>0</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="14">
         <v>0</v>
       </c>
       <c r="G24" s="7">
@@ -2054,13 +2096,13 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="18">
+      <c r="A25" s="14">
         <v>23</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="14">
         <v>3</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="14">
         <v>1</v>
       </c>
       <c r="D25" s="7">
@@ -2069,7 +2111,7 @@
       <c r="E25" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="14">
         <v>0</v>
       </c>
       <c r="G25" s="7">
@@ -2092,10 +2134,10 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="18">
+      <c r="A26" s="14">
         <v>24</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="14">
         <v>3</v>
       </c>
       <c r="C26" s="7">
@@ -2107,7 +2149,7 @@
       <c r="E26" s="7">
         <v>0</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="14">
         <v>0</v>
       </c>
       <c r="G26" s="7">
@@ -2130,13 +2172,13 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="18">
+      <c r="A27" s="14">
         <v>25</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="14">
         <v>3</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="14">
         <v>1</v>
       </c>
       <c r="D27" s="7">
@@ -2145,7 +2187,7 @@
       <c r="E27" s="7">
         <v>0</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="14">
         <v>0</v>
       </c>
       <c r="G27" s="7">
@@ -2168,10 +2210,10 @@
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="18">
+      <c r="A28" s="14">
         <v>26</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="14">
         <v>3</v>
       </c>
       <c r="C28" s="7">
@@ -2180,10 +2222,10 @@
       <c r="D28" s="7">
         <v>0</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="14">
         <v>0</v>
       </c>
       <c r="G28" s="7">
@@ -2206,28 +2248,28 @@
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="39">
+      <c r="A29" s="24">
         <v>27</v>
       </c>
-      <c r="B29" s="39">
+      <c r="B29" s="24">
         <v>3</v>
       </c>
-      <c r="C29" s="39">
-        <v>1</v>
-      </c>
-      <c r="D29" s="40">
-        <v>0</v>
-      </c>
-      <c r="E29" s="41">
+      <c r="C29" s="24">
+        <v>1</v>
+      </c>
+      <c r="D29" s="25">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26">
         <v>2</v>
       </c>
-      <c r="F29" s="39">
-        <v>0</v>
-      </c>
-      <c r="G29" s="40">
+      <c r="F29" s="24">
+        <v>0</v>
+      </c>
+      <c r="G29" s="25">
         <v>2.81</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="25">
         <v>0.76</v>
       </c>
       <c r="I29" s="7">
@@ -2244,10 +2286,10 @@
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="18">
+      <c r="A30" s="14">
         <v>28</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="14">
         <v>3</v>
       </c>
       <c r="C30" s="7">
@@ -2256,10 +2298,10 @@
       <c r="D30" s="7">
         <v>0</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="15">
         <v>2</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="14">
         <v>0</v>
       </c>
       <c r="G30" s="7">
@@ -2282,22 +2324,22 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="18">
+      <c r="A31" s="14">
         <v>29</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="14">
         <v>3</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="14">
         <v>1</v>
       </c>
       <c r="D31" s="7">
         <v>0</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="15">
         <v>2</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="14">
         <v>0</v>
       </c>
       <c r="G31" s="7">
@@ -2320,10 +2362,10 @@
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="18">
+      <c r="A32" s="14">
         <v>30</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="14">
         <v>3</v>
       </c>
       <c r="C32" s="7">
@@ -2335,7 +2377,7 @@
       <c r="E32" s="7">
         <v>0</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="14">
         <v>0</v>
       </c>
       <c r="G32" s="7">
@@ -2364,7 +2406,7 @@
       <c r="B33" s="7">
         <v>3</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="14">
         <v>1</v>
       </c>
       <c r="D33" s="7">
@@ -2373,7 +2415,7 @@
       <c r="E33" s="7">
         <v>0</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="14">
         <v>0</v>
       </c>
       <c r="G33" s="7">
@@ -2402,7 +2444,7 @@
       <c r="B34" s="7">
         <v>3</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="14">
         <v>1</v>
       </c>
       <c r="D34" s="7">
@@ -2411,7 +2453,7 @@
       <c r="E34" s="7">
         <v>0</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="14">
         <v>0</v>
       </c>
       <c r="G34" s="7">
@@ -2440,7 +2482,7 @@
       <c r="B35" s="7">
         <v>3</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="14">
         <v>1</v>
       </c>
       <c r="D35" s="7">
@@ -2449,7 +2491,7 @@
       <c r="E35" s="7">
         <v>0</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="14">
         <v>0</v>
       </c>
       <c r="G35" s="7">
@@ -2487,7 +2529,7 @@
       <c r="E36" s="7">
         <v>1</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="14">
         <v>0</v>
       </c>
       <c r="G36" s="7">
@@ -2516,16 +2558,16 @@
       <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="14">
         <v>1</v>
       </c>
       <c r="D37" s="7">
         <v>0</v>
       </c>
-      <c r="E37" s="42">
+      <c r="E37" s="27">
         <v>2</v>
       </c>
-      <c r="F37" s="43">
+      <c r="F37" s="28">
         <v>0</v>
       </c>
       <c r="G37" s="7">
@@ -2563,7 +2605,7 @@
       <c r="E38" s="7">
         <v>0</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="14">
         <v>0</v>
       </c>
       <c r="G38" s="7">
@@ -2592,7 +2634,7 @@
       <c r="B39" s="7">
         <v>3</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="14">
         <v>1</v>
       </c>
       <c r="D39" s="7">
@@ -2601,7 +2643,7 @@
       <c r="E39" s="7">
         <v>0</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="14">
         <v>0</v>
       </c>
       <c r="G39" s="7">
@@ -2639,7 +2681,7 @@
       <c r="E40" s="7">
         <v>0</v>
       </c>
-      <c r="F40" s="18">
+      <c r="F40" s="14">
         <v>0</v>
       </c>
       <c r="G40" s="7">
@@ -2668,16 +2710,16 @@
       <c r="B41" s="7">
         <v>3</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="14">
         <v>1</v>
       </c>
       <c r="D41" s="7">
         <v>0</v>
       </c>
-      <c r="E41" s="42">
+      <c r="E41" s="27">
         <v>2</v>
       </c>
-      <c r="F41" s="43">
+      <c r="F41" s="28">
         <v>0</v>
       </c>
       <c r="G41" s="7">
@@ -2715,7 +2757,7 @@
       <c r="E42" s="7">
         <v>0</v>
       </c>
-      <c r="F42" s="18">
+      <c r="F42" s="14">
         <v>0</v>
       </c>
       <c r="G42" s="7">
@@ -2744,7 +2786,7 @@
       <c r="B43" s="7">
         <v>3</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="14">
         <v>1</v>
       </c>
       <c r="D43" s="7">
@@ -2753,7 +2795,7 @@
       <c r="E43" s="7">
         <v>0</v>
       </c>
-      <c r="F43" s="18">
+      <c r="F43" s="14">
         <v>0</v>
       </c>
       <c r="G43" s="7">
@@ -2791,7 +2833,7 @@
       <c r="E44" s="7">
         <v>0</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="14">
         <v>0</v>
       </c>
       <c r="G44" s="7">
@@ -2820,16 +2862,16 @@
       <c r="B45" s="7">
         <v>3</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="14">
         <v>1</v>
       </c>
       <c r="D45" s="7">
         <v>0</v>
       </c>
-      <c r="E45" s="42">
+      <c r="E45" s="27">
         <v>2</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="28">
         <v>0</v>
       </c>
       <c r="G45" s="7">
@@ -2864,10 +2906,10 @@
       <c r="D46" s="7">
         <v>0</v>
       </c>
-      <c r="E46" s="42">
+      <c r="E46" s="27">
         <v>2</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="28">
         <v>0</v>
       </c>
       <c r="G46" s="7">
@@ -2896,16 +2938,16 @@
       <c r="B47" s="7">
         <v>3</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="14">
         <v>1</v>
       </c>
       <c r="D47" s="7">
         <v>0</v>
       </c>
-      <c r="E47" s="42">
+      <c r="E47" s="27">
         <v>2</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="28">
         <v>0</v>
       </c>
       <c r="G47" s="7">
@@ -2943,7 +2985,7 @@
       <c r="E48" s="7">
         <v>0</v>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="14">
         <v>0</v>
       </c>
       <c r="G48" s="7">
@@ -2972,7 +3014,7 @@
       <c r="B49" s="7">
         <v>3</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="14">
         <v>1</v>
       </c>
       <c r="D49" s="7">
@@ -2981,7 +3023,7 @@
       <c r="E49" s="7">
         <v>0</v>
       </c>
-      <c r="F49" s="18">
+      <c r="F49" s="14">
         <v>0</v>
       </c>
       <c r="G49" s="7">
@@ -3019,7 +3061,7 @@
       <c r="E50" s="7">
         <v>0</v>
       </c>
-      <c r="F50" s="18">
+      <c r="F50" s="14">
         <v>0</v>
       </c>
       <c r="G50" s="7">
@@ -3048,7 +3090,7 @@
       <c r="B51" s="7">
         <v>3</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="14">
         <v>1</v>
       </c>
       <c r="D51" s="7">
@@ -3057,7 +3099,7 @@
       <c r="E51" s="7">
         <v>0</v>
       </c>
-      <c r="F51" s="18">
+      <c r="F51" s="14">
         <v>0</v>
       </c>
       <c r="G51" s="7">
@@ -3092,10 +3134,10 @@
       <c r="D52" s="7">
         <v>0</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="27">
         <v>2</v>
       </c>
-      <c r="F52" s="43">
+      <c r="F52" s="28">
         <v>0</v>
       </c>
       <c r="G52" s="7">
@@ -3124,16 +3166,16 @@
       <c r="B53" s="7">
         <v>3</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="14">
         <v>1</v>
       </c>
       <c r="D53" s="7">
         <v>0</v>
       </c>
-      <c r="E53" s="42">
+      <c r="E53" s="27">
         <v>2</v>
       </c>
-      <c r="F53" s="43">
+      <c r="F53" s="28">
         <v>0</v>
       </c>
       <c r="G53" s="7">
@@ -3171,7 +3213,7 @@
       <c r="E54" s="7">
         <v>0</v>
       </c>
-      <c r="F54" s="18">
+      <c r="F54" s="14">
         <v>0</v>
       </c>
       <c r="G54" s="7">
@@ -3200,7 +3242,7 @@
       <c r="B55" s="7">
         <v>3</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="14">
         <v>1</v>
       </c>
       <c r="D55" s="7">
@@ -3209,7 +3251,7 @@
       <c r="E55" s="7">
         <v>0</v>
       </c>
-      <c r="F55" s="18">
+      <c r="F55" s="14">
         <v>0</v>
       </c>
       <c r="G55" s="7">
@@ -3247,7 +3289,7 @@
       <c r="E56" s="7">
         <v>0</v>
       </c>
-      <c r="F56" s="18">
+      <c r="F56" s="14">
         <v>0</v>
       </c>
       <c r="G56" s="7">
@@ -3276,7 +3318,7 @@
       <c r="B57" s="7">
         <v>3</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="14">
         <v>1</v>
       </c>
       <c r="D57" s="7">
@@ -3285,7 +3327,7 @@
       <c r="E57" s="7">
         <v>0</v>
       </c>
-      <c r="F57" s="18">
+      <c r="F57" s="14">
         <v>0</v>
       </c>
       <c r="G57" s="7">
@@ -3323,7 +3365,7 @@
       <c r="E58" s="7">
         <v>0</v>
       </c>
-      <c r="F58" s="18">
+      <c r="F58" s="14">
         <v>0</v>
       </c>
       <c r="G58" s="7">
@@ -3352,7 +3394,7 @@
       <c r="B59" s="7">
         <v>3</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="14">
         <v>1</v>
       </c>
       <c r="D59" s="7">
@@ -3361,7 +3403,7 @@
       <c r="E59" s="7">
         <v>0</v>
       </c>
-      <c r="F59" s="18">
+      <c r="F59" s="14">
         <v>0</v>
       </c>
       <c r="G59" s="7">
@@ -3396,7 +3438,7 @@
       <c r="D60">
         <v>0</v>
       </c>
-      <c r="E60" s="19">
+      <c r="E60" s="15">
         <v>1</v>
       </c>
       <c r="F60">
@@ -3434,7 +3476,7 @@
       <c r="D61">
         <v>0</v>
       </c>
-      <c r="E61" s="19">
+      <c r="E61" s="15">
         <v>1</v>
       </c>
       <c r="F61">
@@ -3813,8 +3855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AQ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3846,9 +3888,8 @@
     </row>
     <row r="2" spans="1:43">
       <c r="A2" s="3"/>
-      <c r="C2" s="36" t="s">
-        <v>58</v>
-      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -3862,343 +3903,307 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="38" t="s">
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-    </row>
-    <row r="3" spans="1:43" s="13" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="C3" s="14" t="s">
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+    </row>
+    <row r="3" spans="1:43" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AB3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AC3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AD3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AE3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" s="15" t="s">
+      <c r="AF3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AG3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="AH3" s="16" t="s">
+      <c r="AH3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="AJ3" s="16" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="AK3" s="16" t="s">
+      <c r="AK3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AL3" s="16" t="s">
+      <c r="AL3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AM3" s="16" t="s">
+      <c r="AM3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AN3" s="16" t="s">
+      <c r="AN3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AO3" s="16" t="s">
+      <c r="AO3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AP3" s="16" t="s">
+      <c r="AP3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AQ3" s="16" t="s">
+      <c r="AQ3" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="13" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="1:43" s="38" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A4" s="37"/>
+      <c r="B4" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-    </row>
-    <row r="5" spans="1:43" s="13" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="C5" t="s">
+      <c r="C4" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D4" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E4" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F4" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G4" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H4" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I4" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J4" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K4" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L4" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
-      <c r="AO5" s="16"/>
-      <c r="AP5" s="16"/>
-      <c r="AQ5" s="16"/>
-    </row>
-    <row r="6" spans="1:43" s="28" customFormat="1">
-      <c r="A6" s="20">
-        <v>1</v>
-      </c>
-      <c r="B6" s="20">
+      <c r="M4" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" s="38" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A5" s="37"/>
+      <c r="B5" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:43" s="32" customFormat="1">
+      <c r="A6" s="30">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30">
         <v>38</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="31">
         <v>2.0500000000000002E-3</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="31">
         <f>C6*2</f>
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="31">
         <v>1.78E-2</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="31">
         <v>3.5500000000000002E-3</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="31">
         <v>2.7499999999999998E-3</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="32">
         <v>7.8</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="32">
         <v>0.05</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="32">
         <v>1.67E-2</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="32">
         <v>4.7499999999999999E-3</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="32">
         <v>2.7499999999999998E-3</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="32">
         <v>1.5</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="32">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="32">
         <v>450</v>
       </c>
-      <c r="P6" s="27">
+      <c r="P6" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:43">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="33">
         <v>39</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="35">
         <f t="shared" ref="D7:D19" si="0">C7*2</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="18">
         <v>0.29499999999999998</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="18">
         <v>6.9699999999999998E-2</v>
       </c>
       <c r="G7" s="8">
@@ -4314,23 +4319,23 @@
       </c>
     </row>
     <row r="8" spans="1:43">
-      <c r="A8" s="18">
+      <c r="A8" s="14">
         <v>3</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="33">
         <v>39</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="18">
         <v>3.04E-2</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="35">
         <f t="shared" si="0"/>
         <v>6.08E-2</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="18">
         <v>0.2495</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="18">
         <v>5.3100000000000001E-2</v>
       </c>
       <c r="G8" s="8">
@@ -4446,23 +4451,23 @@
       </c>
     </row>
     <row r="9" spans="1:43">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>4</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="33">
         <v>39</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="18">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="35">
         <f t="shared" si="0"/>
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="18">
         <v>0.26200000000000001</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="18">
         <v>4.36E-2</v>
       </c>
       <c r="G9" s="8">
@@ -4578,23 +4583,23 @@
       </c>
     </row>
     <row r="10" spans="1:43">
-      <c r="A10" s="18">
+      <c r="A10" s="14">
         <v>5</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="33">
         <v>39</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="18">
         <v>2.7E-2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="35">
         <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="18">
         <v>0.33</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="18">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="G10" s="8">
@@ -4710,23 +4715,23 @@
       </c>
     </row>
     <row r="11" spans="1:43">
-      <c r="A11" s="18">
+      <c r="A11" s="14">
         <v>6</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="33">
         <v>39</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="18">
         <v>2.24E-2</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="35">
         <f t="shared" si="0"/>
         <v>4.48E-2</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="18">
         <v>0.254</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="18">
         <v>0.05</v>
       </c>
       <c r="G11" s="8">
@@ -4842,23 +4847,23 @@
       </c>
     </row>
     <row r="12" spans="1:43">
-      <c r="A12" s="18">
+      <c r="A12" s="14">
         <v>7</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="33">
         <v>39</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="18">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="35">
         <f t="shared" si="0"/>
         <v>6.4399999999999999E-2</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="18">
         <v>0.29499999999999998</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="18">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="G12" s="8">
@@ -4974,23 +4979,23 @@
       </c>
     </row>
     <row r="13" spans="1:43">
-      <c r="A13" s="18">
+      <c r="A13" s="14">
         <v>8</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="33">
         <v>39</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="18">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="35">
         <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="18">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G13" s="8">
@@ -5106,41 +5111,44 @@
       </c>
     </row>
     <row r="14" spans="1:43">
-      <c r="A14" s="18">
+      <c r="A14" s="51">
         <v>9</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="50">
         <v>28</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="42">
         <v>0.04</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="42">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="42">
         <v>0.03</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="42">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="42">
         <v>4.7750000000000002E-5</v>
       </c>
-      <c r="H14" s="32">
-        <v>0</v>
-      </c>
-      <c r="I14" s="32">
+      <c r="H14" s="43">
+        <v>0</v>
+      </c>
+      <c r="I14" s="43">
         <v>1E-3</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="43">
         <v>20</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="43">
         <v>100</v>
       </c>
-      <c r="L14" s="32">
+      <c r="L14" s="43">
         <v>250</v>
+      </c>
+      <c r="M14" s="43">
+        <v>1</v>
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
@@ -5170,23 +5178,23 @@
       <c r="AQ14" s="7"/>
     </row>
     <row r="15" spans="1:43">
-      <c r="A15" s="18">
+      <c r="A15" s="14">
         <v>10</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="33">
         <v>39</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="18">
         <v>1.9900000000000001E-2</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="35">
         <f t="shared" si="0"/>
         <v>3.9800000000000002E-2</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="18">
         <v>0.16900000000000001</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="18">
         <v>4.5699999999999998E-2</v>
       </c>
       <c r="G15" s="8">
@@ -5302,23 +5310,23 @@
       </c>
     </row>
     <row r="16" spans="1:43">
-      <c r="A16" s="18">
+      <c r="A16" s="14">
         <v>11</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="33">
         <v>39</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="18">
         <v>1.03E-2</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="35">
         <f t="shared" si="0"/>
         <v>2.06E-2</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="18">
         <v>0.128</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="18">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="G16" s="8">
@@ -5384,7 +5392,7 @@
       <c r="AA16" s="7">
         <v>0.91</v>
       </c>
-      <c r="AB16" s="30">
+      <c r="AB16" s="19">
         <v>0.03</v>
       </c>
       <c r="AC16" s="7">
@@ -5434,32 +5442,35 @@
       </c>
     </row>
     <row r="17" spans="1:43">
-      <c r="A17" s="18">
+      <c r="A17" s="47">
         <v>12</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="48">
         <v>18</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="49">
         <v>2.5</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="49">
         <v>7.5</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="49">
         <v>20</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="49">
         <v>20</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="49">
         <v>500</v>
+      </c>
+      <c r="J17" s="49">
+        <v>1.2</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
@@ -5488,66 +5499,65 @@
       <c r="AP17" s="7"/>
       <c r="AQ17" s="7"/>
     </row>
-    <row r="18" spans="1:43">
-      <c r="A18" s="22">
+    <row r="18" spans="1:43" s="36" customFormat="1">
+      <c r="A18" s="51">
         <v>13</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="50">
         <v>28</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="43">
         <v>0.04</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="43">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="43">
         <v>0.4</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="43">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="43">
         <v>9.55E-6</v>
       </c>
-      <c r="H18" s="32">
-        <v>0</v>
-      </c>
-      <c r="I18" s="45">
+      <c r="H18" s="43">
+        <v>0</v>
+      </c>
+      <c r="I18" s="43">
         <v>1E-3</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="43">
         <v>20</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="43">
         <v>100</v>
       </c>
-      <c r="L18" s="32">
+      <c r="L18" s="43">
         <v>150</v>
       </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
+      <c r="M18" s="43">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:43">
-      <c r="A19" s="18">
+      <c r="A19" s="14">
         <v>14</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="33">
         <v>38</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="18">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="35">
         <f t="shared" si="0"/>
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="18">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="18">
         <v>2.8500000000000001E-3</v>
       </c>
       <c r="G19" s="8">
@@ -5582,950 +5592,998 @@
       </c>
     </row>
     <row r="20" spans="1:43">
-      <c r="A20" s="23">
+      <c r="A20" s="50">
         <v>15</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="50">
         <v>28</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="43">
         <v>0.2</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="43">
         <v>0.02</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="43">
         <v>0.08</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="43">
         <v>0.03</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="43">
         <v>9.55E-6</v>
       </c>
-      <c r="H20" s="32">
-        <v>0</v>
-      </c>
-      <c r="I20" s="33">
+      <c r="H20" s="43">
+        <v>0</v>
+      </c>
+      <c r="I20" s="43">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="J20" s="32">
+      <c r="J20" s="43">
         <v>20</v>
       </c>
-      <c r="K20" s="32">
+      <c r="K20" s="43">
         <v>100</v>
       </c>
-      <c r="L20" s="32">
+      <c r="L20" s="43">
         <v>150</v>
       </c>
-    </row>
-    <row r="21" spans="1:43" s="28" customFormat="1">
-      <c r="A21" s="24">
+      <c r="M20" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" s="17" customFormat="1">
+      <c r="A21" s="16">
         <v>16</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="34">
         <v>39</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="21">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="35">
         <f>C21*2</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="21">
         <v>0.1</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="21">
         <v>3.1E-2</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="17">
         <v>10.199999999999999</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="17">
         <v>0.05</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="17">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="17">
         <v>4.1666700000000001E-2</v>
       </c>
-      <c r="L21" s="28">
+      <c r="L21" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M21" s="28">
+      <c r="M21" s="17">
         <v>1.5</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="17">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="O21" s="28">
+      <c r="O21" s="17">
         <v>42</v>
       </c>
-      <c r="P21" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="28">
+      <c r="P21" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="17">
         <v>0.01</v>
       </c>
-      <c r="R21" s="28">
-        <v>1</v>
-      </c>
-      <c r="S21" s="28">
+      <c r="R21" s="17">
+        <v>1</v>
+      </c>
+      <c r="S21" s="17">
         <v>0.02</v>
       </c>
-      <c r="T21" s="28">
+      <c r="T21" s="17">
         <v>10</v>
       </c>
-      <c r="U21" s="28">
+      <c r="U21" s="17">
         <v>-10</v>
       </c>
-      <c r="V21" s="28">
-        <v>1</v>
-      </c>
-      <c r="W21" s="28">
+      <c r="V21" s="17">
+        <v>1</v>
+      </c>
+      <c r="W21" s="17">
         <v>0.78500000000000003</v>
       </c>
-      <c r="X21" s="28">
+      <c r="X21" s="17">
         <v>3.9266999999999999</v>
       </c>
-      <c r="Y21" s="28">
+      <c r="Y21" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Z21" s="28">
+      <c r="Z21" s="17">
         <v>5.2355999999999998</v>
       </c>
-      <c r="AA21" s="28">
+      <c r="AA21" s="17">
         <v>0.91</v>
       </c>
-      <c r="AB21" s="28">
+      <c r="AB21" s="17">
         <v>0.03</v>
       </c>
-      <c r="AC21" s="28">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="28">
+      <c r="AC21" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="17">
         <v>200</v>
       </c>
-      <c r="AE21" s="28">
+      <c r="AE21" s="17">
         <v>50</v>
       </c>
-      <c r="AF21" s="28">
+      <c r="AF21" s="17">
         <v>50</v>
       </c>
-      <c r="AG21" s="28">
+      <c r="AG21" s="17">
         <v>0.01</v>
       </c>
-      <c r="AH21" s="28">
+      <c r="AH21" s="17">
         <v>20</v>
       </c>
-      <c r="AI21" s="28">
+      <c r="AI21" s="17">
         <v>15</v>
       </c>
-      <c r="AJ21" s="28">
+      <c r="AJ21" s="17">
         <v>0.15</v>
       </c>
-      <c r="AK21" s="28">
+      <c r="AK21" s="17">
         <v>0.04</v>
       </c>
-      <c r="AL21" s="28">
+      <c r="AL21" s="17">
         <v>0.15</v>
       </c>
-      <c r="AM21" s="28">
+      <c r="AM21" s="17">
         <v>0.04</v>
       </c>
-      <c r="AN21" s="28">
+      <c r="AN21" s="17">
         <v>0.15</v>
       </c>
-      <c r="AO21" s="28">
+      <c r="AO21" s="17">
         <v>0.04</v>
       </c>
-      <c r="AP21" s="28">
+      <c r="AP21" s="17">
         <v>0.2</v>
       </c>
-      <c r="AQ21" s="28">
+      <c r="AQ21" s="17">
         <v>-0.05</v>
       </c>
     </row>
     <row r="22" spans="1:43">
-      <c r="A22" s="18">
+      <c r="A22" s="47">
         <v>17</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="48">
         <v>18</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="49">
         <v>2.5</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="49">
         <v>7.5</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="49">
         <v>20</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="49">
         <v>20</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="49">
         <v>500</v>
       </c>
+      <c r="J22" s="46">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:43">
-      <c r="A23" s="18">
+      <c r="A23" s="14">
         <v>18</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="14">
         <v>100</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:43">
-      <c r="A24" s="18">
+      <c r="A24" s="14">
         <v>19</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:43">
-      <c r="A25" s="18">
+      <c r="A25" s="14">
         <v>20</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:43">
-      <c r="A26" s="18">
+      <c r="A26" s="14">
         <v>21</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:43">
-      <c r="A27" s="18">
+      <c r="A27" s="14">
         <v>22</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:43">
-      <c r="A28" s="18">
+      <c r="A28" s="14">
         <v>23</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:43">
-      <c r="A29" s="18">
+      <c r="A29" s="14">
         <v>24</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:43">
-      <c r="A30" s="18">
+      <c r="A30" s="14">
         <v>25</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="14">
         <v>100</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:43">
-      <c r="A31" s="18">
+      <c r="A31" s="47">
         <v>26</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="47">
         <v>18</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="49">
         <v>2.5</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="49">
         <v>7.5</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F31" s="32">
+      <c r="F31" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G31" s="32">
+      <c r="G31" s="49">
         <v>20</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="49">
         <v>20</v>
       </c>
-      <c r="I31" s="32">
+      <c r="I31" s="49">
         <v>400</v>
       </c>
+      <c r="J31" s="49">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:43">
-      <c r="A32" s="18">
+      <c r="A32" s="47">
         <v>27</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="48">
         <v>18</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="49">
         <v>2.5</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="49">
         <v>7.5</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G32" s="49">
         <v>20</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="49">
         <v>20</v>
       </c>
-      <c r="I32" s="33">
+      <c r="I32" s="49">
         <v>350</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="18">
+      <c r="J32" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="47">
         <v>28</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="48">
         <v>18</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="49">
         <v>2.5</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="49">
         <v>7.5</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F33" s="32">
+      <c r="F33" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G33" s="49">
         <v>20</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="49">
         <v>20</v>
       </c>
-      <c r="I33" s="33">
+      <c r="I33" s="49">
         <v>350</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="18">
+      <c r="J33" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="47">
         <v>29</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="47">
         <v>18</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="49">
         <v>2.5</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="49">
         <v>7.5</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F34" s="32">
+      <c r="F34" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="49">
         <v>20</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="49">
         <v>20</v>
       </c>
-      <c r="I34" s="33">
+      <c r="I34" s="49">
         <v>400</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="18">
+      <c r="J34" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="14">
         <v>30</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="14">
         <v>100</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="7">
         <v>31</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="14">
         <v>100</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="7">
         <v>32</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="14">
         <v>100</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="7">
         <v>33</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="14">
         <v>100</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="7">
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="52">
         <v>34</v>
       </c>
-      <c r="B39" s="23">
+      <c r="B39" s="50">
         <v>28</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="43">
         <v>0.2</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="43">
         <v>0.02</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="43">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F39" s="43">
+        <v>0.02</v>
+      </c>
+      <c r="G39" s="43">
+        <v>9.55E-6</v>
+      </c>
+      <c r="H39" s="43">
+        <v>0</v>
+      </c>
+      <c r="I39" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="J39" s="43">
+        <v>20</v>
+      </c>
+      <c r="K39" s="43">
+        <v>150</v>
+      </c>
+      <c r="L39" s="43">
+        <v>400</v>
+      </c>
+      <c r="M39" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="53">
+        <v>35</v>
+      </c>
+      <c r="B40" s="48">
+        <v>18</v>
+      </c>
+      <c r="C40" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="D40" s="49">
+        <v>7.5</v>
+      </c>
+      <c r="E40" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F39" s="32">
-        <v>0.02</v>
-      </c>
-      <c r="G39" s="32">
-        <v>9.55E-6</v>
-      </c>
-      <c r="H39" s="32">
-        <v>0</v>
-      </c>
-      <c r="I39" s="45">
-        <v>1E-4</v>
-      </c>
-      <c r="J39" s="32">
+      <c r="F40" s="49">
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="G40" s="49">
         <v>20</v>
       </c>
-      <c r="K39" s="32">
-        <v>150</v>
-      </c>
-      <c r="L39" s="32">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="7">
-        <v>35</v>
-      </c>
-      <c r="B40" s="23">
-        <v>18</v>
-      </c>
-      <c r="C40" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="D40" s="32">
-        <v>7.5</v>
-      </c>
-      <c r="E40" s="32">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F40" s="32">
-        <v>1.6666666666666668E-3</v>
-      </c>
-      <c r="G40" s="32">
+      <c r="H40" s="49">
         <v>20</v>
       </c>
-      <c r="H40" s="32">
-        <v>20</v>
-      </c>
-      <c r="I40" s="32">
+      <c r="I40" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="J40" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="7">
         <v>36</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13">
       <c r="A42" s="7">
         <v>37</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13">
       <c r="A43" s="7">
         <v>38</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="14">
         <v>100</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="7">
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="53">
         <v>39</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="48">
         <v>18</v>
       </c>
-      <c r="C44" s="32">
+      <c r="C44" s="49">
         <v>2.5</v>
       </c>
-      <c r="D44" s="32">
+      <c r="D44" s="49">
         <v>7.5</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F44" s="32">
+      <c r="F44" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G44" s="32">
+      <c r="G44" s="49">
         <v>20</v>
       </c>
-      <c r="H44" s="32">
+      <c r="H44" s="49">
         <v>20</v>
       </c>
-      <c r="I44" s="32">
+      <c r="I44" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="J44" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="7">
         <v>40</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:13">
       <c r="A46" s="7">
         <v>41</v>
       </c>
-      <c r="B46" s="18">
+      <c r="B46" s="14">
         <v>100</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="7">
         <v>42</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="7">
+    <row r="48" spans="1:13">
+      <c r="A48" s="53">
         <v>43</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="48">
         <v>18</v>
       </c>
-      <c r="C48" s="32">
+      <c r="C48" s="49">
         <v>2.5</v>
       </c>
-      <c r="D48" s="32">
+      <c r="D48" s="49">
         <v>7.5</v>
       </c>
-      <c r="E48" s="32">
+      <c r="E48" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F48" s="32">
+      <c r="F48" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G48" s="32">
+      <c r="G48" s="49">
         <v>20</v>
       </c>
-      <c r="H48" s="32">
+      <c r="H48" s="49">
         <v>20</v>
       </c>
-      <c r="I48" s="32">
+      <c r="I48" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="7">
+      <c r="J48" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="53">
         <v>44</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="48">
         <v>18</v>
       </c>
-      <c r="C49" s="32">
+      <c r="C49" s="49">
         <v>2.5</v>
       </c>
-      <c r="D49" s="32">
+      <c r="D49" s="49">
         <v>7.5</v>
       </c>
-      <c r="E49" s="32">
+      <c r="E49" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F49" s="32">
+      <c r="F49" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G49" s="32">
+      <c r="G49" s="49">
         <v>20</v>
       </c>
-      <c r="H49" s="32">
+      <c r="H49" s="49">
         <v>20</v>
       </c>
-      <c r="I49" s="32">
+      <c r="I49" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="7">
+      <c r="J49" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="53">
         <v>45</v>
       </c>
-      <c r="B50" s="23">
+      <c r="B50" s="48">
         <v>18</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="49">
         <v>2.5</v>
       </c>
-      <c r="D50" s="32">
+      <c r="D50" s="49">
         <v>7.5</v>
       </c>
-      <c r="E50" s="32">
+      <c r="E50" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F50" s="32">
+      <c r="F50" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G50" s="32">
+      <c r="G50" s="49">
         <v>20</v>
       </c>
-      <c r="H50" s="32">
+      <c r="H50" s="49">
         <v>20</v>
       </c>
-      <c r="I50" s="32">
+      <c r="I50" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="7">
         <v>46</v>
       </c>
-      <c r="B51" s="18">
+      <c r="B51" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:10">
       <c r="A52" s="7">
         <v>47</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:10">
       <c r="A53" s="7">
         <v>48</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B53" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:10">
       <c r="A54" s="7">
         <v>49</v>
       </c>
-      <c r="B54" s="18">
+      <c r="B54" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="7">
+    <row r="55" spans="1:10">
+      <c r="A55" s="53">
         <v>50</v>
       </c>
-      <c r="B55" s="23">
+      <c r="B55" s="48">
         <v>18</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="49">
         <v>2.5</v>
       </c>
-      <c r="D55" s="32">
+      <c r="D55" s="49">
         <v>7.5</v>
       </c>
-      <c r="E55" s="32">
+      <c r="E55" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F55" s="32">
+      <c r="F55" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G55" s="32">
+      <c r="G55" s="49">
         <v>20</v>
       </c>
-      <c r="H55" s="32">
+      <c r="H55" s="49">
         <v>20</v>
       </c>
-      <c r="I55" s="32">
+      <c r="I55" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="7">
+      <c r="J55" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="53">
         <v>51</v>
       </c>
-      <c r="B56" s="23">
+      <c r="B56" s="48">
         <v>18</v>
       </c>
-      <c r="C56" s="32">
+      <c r="C56" s="49">
         <v>2.5</v>
       </c>
-      <c r="D56" s="32">
+      <c r="D56" s="49">
         <v>7.5</v>
       </c>
-      <c r="E56" s="32">
+      <c r="E56" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F56" s="32">
+      <c r="F56" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G56" s="32">
+      <c r="G56" s="49">
         <v>20</v>
       </c>
-      <c r="H56" s="32">
+      <c r="H56" s="49">
         <v>20</v>
       </c>
-      <c r="I56" s="32">
+      <c r="I56" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="7">
         <v>52</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="14">
         <v>100</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="7">
         <v>53</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B58" s="14">
         <v>100</v>
       </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="7">
         <v>54</v>
       </c>
-      <c r="B59" s="18">
+      <c r="B59" s="14">
         <v>100</v>
       </c>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="35"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="22"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="7">
         <v>55</v>
       </c>
-      <c r="B60" s="18">
+      <c r="B60" s="14">
         <v>100</v>
       </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="7">
         <v>56</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:10">
       <c r="A62" s="7">
         <v>57</v>
       </c>
-      <c r="B62" s="18">
+      <c r="B62" s="14">
         <v>100</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63">
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="46">
         <v>58</v>
       </c>
-      <c r="B63" s="23">
+      <c r="B63" s="48">
         <v>18</v>
       </c>
-      <c r="C63" s="32">
+      <c r="C63" s="49">
         <v>2.5</v>
       </c>
-      <c r="D63" s="32">
+      <c r="D63" s="49">
         <v>7.5</v>
       </c>
-      <c r="E63" s="32">
+      <c r="E63" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F63" s="32">
+      <c r="F63" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G63" s="32">
+      <c r="G63" s="49">
         <v>20</v>
       </c>
-      <c r="H63" s="32">
+      <c r="H63" s="49">
         <v>20</v>
       </c>
-      <c r="I63" s="32">
+      <c r="I63" s="49">
         <v>500</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64">
+      <c r="J63" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="46">
         <v>59</v>
       </c>
-      <c r="B64" s="23">
+      <c r="B64" s="48">
         <v>18</v>
       </c>
-      <c r="C64" s="32">
+      <c r="C64" s="49">
         <v>2.5</v>
       </c>
-      <c r="D64" s="32">
+      <c r="D64" s="49">
         <v>7.5</v>
       </c>
-      <c r="E64" s="32">
+      <c r="E64" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F64" s="32">
+      <c r="F64" s="49">
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="G64" s="32">
+      <c r="G64" s="49">
         <v>20</v>
       </c>
-      <c r="H64" s="32">
+      <c r="H64" s="49">
         <v>20</v>
       </c>
-      <c r="I64" s="32">
+      <c r="I64" s="49">
         <v>500</v>
+      </c>
+      <c r="J64" s="49">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
         <v>60</v>
       </c>
-      <c r="B65" s="18">
+      <c r="B65" s="14">
         <v>100</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
         <v>61</v>
       </c>
-      <c r="B66" s="18">
+      <c r="B66" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6533,7 +6591,7 @@
       <c r="A67">
         <v>62</v>
       </c>
-      <c r="B67" s="18">
+      <c r="B67" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6541,7 +6599,7 @@
       <c r="A68">
         <v>63</v>
       </c>
-      <c r="B68" s="18">
+      <c r="B68" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6549,7 +6607,7 @@
       <c r="A69">
         <v>64</v>
       </c>
-      <c r="B69" s="18">
+      <c r="B69" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6557,7 +6615,7 @@
       <c r="A70">
         <v>65</v>
       </c>
-      <c r="B70" s="18">
+      <c r="B70" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6565,7 +6623,7 @@
       <c r="A71">
         <v>66</v>
       </c>
-      <c r="B71" s="18">
+      <c r="B71" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6573,7 +6631,7 @@
       <c r="A72">
         <v>67</v>
       </c>
-      <c r="B72" s="18">
+      <c r="B72" s="14">
         <v>100</v>
       </c>
     </row>
@@ -6581,16 +6639,16 @@
       <c r="A73">
         <v>68</v>
       </c>
-      <c r="B73" s="18">
+      <c r="B73" s="14">
         <v>100</v>
       </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6665,7 +6723,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>